<commit_message>
Updated to latest data model
</commit_message>
<xml_diff>
--- a/datatemplate.xlsx
+++ b/datatemplate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>PetID</t>
   </si>
@@ -36,6 +36,12 @@
     <t>age</t>
   </si>
   <si>
+    <t>Fido</t>
+  </si>
+  <si>
+    <t>Meowster</t>
+  </si>
+  <si>
     <t>Ruffy</t>
   </si>
   <si>
@@ -51,6 +57,12 @@
     <t>Goldy</t>
   </si>
   <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
     <t>Khali</t>
   </si>
   <si>
@@ -63,7 +75,55 @@
     <t>F</t>
   </si>
   <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
     <t>Woofy</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>abcd1234</t>
+  </si>
+  <si>
+    <t>jvasallo</t>
+  </si>
+  <si>
+    <t>cyoung</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>jvasallo@test.com</t>
+  </si>
+  <si>
+    <t>cyoung@test.com</t>
+  </si>
+  <si>
+    <t>shelter</t>
+  </si>
+  <si>
+    <t>Safe Haven</t>
+  </si>
+  <si>
+    <t>First Woof</t>
+  </si>
+  <si>
+    <t>North Pets</t>
   </si>
 </sst>
 </file>
@@ -413,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A2" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,70 +511,70 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -523,40 +583,40 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -568,65 +628,195 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="F9">
-        <v>5</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E23" r:id="rId1"/>
+    <hyperlink ref="E22" r:id="rId2"/>
+    <hyperlink ref="E21" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>